<commit_message>
data for data-driven tests
</commit_message>
<xml_diff>
--- a/FirstProject/data/pet-store-data.xlsx
+++ b/FirstProject/data/pet-store-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="622">
   <si>
     <t>ITEM_ID</t>
   </si>
@@ -1410,12 +1410,484 @@
   </si>
   <si>
     <t>https://petstore.octoperf.com/actions/Catalog.action?viewItem=&amp;itemId=EST-13</t>
+  </si>
+  <si>
+    <t>5eb869d</t>
+  </si>
+  <si>
+    <t>cf95b1b</t>
+  </si>
+  <si>
+    <t>0861e20</t>
+  </si>
+  <si>
+    <t>a6b4880</t>
+  </si>
+  <si>
+    <t>e12c306</t>
+  </si>
+  <si>
+    <t>4e7991c</t>
+  </si>
+  <si>
+    <t>69c81ff</t>
+  </si>
+  <si>
+    <t>41f49cb</t>
+  </si>
+  <si>
+    <t>49d967f</t>
+  </si>
+  <si>
+    <t>08dad0f</t>
+  </si>
+  <si>
+    <t>6f99d5e</t>
+  </si>
+  <si>
+    <t>403364e</t>
+  </si>
+  <si>
+    <t>91494bb</t>
+  </si>
+  <si>
+    <t>6feaf05</t>
+  </si>
+  <si>
+    <t>5712ad0</t>
+  </si>
+  <si>
+    <t>70c03cd</t>
+  </si>
+  <si>
+    <t>1f3b8eb</t>
+  </si>
+  <si>
+    <t>9dfc60f</t>
+  </si>
+  <si>
+    <t>094beaa</t>
+  </si>
+  <si>
+    <t>e677574</t>
+  </si>
+  <si>
+    <t>f434609</t>
+  </si>
+  <si>
+    <t>69222e5</t>
+  </si>
+  <si>
+    <t>c984835</t>
+  </si>
+  <si>
+    <t>1098856</t>
+  </si>
+  <si>
+    <t>d5cae9e</t>
+  </si>
+  <si>
+    <t>a7cc533</t>
+  </si>
+  <si>
+    <t>eb41f40</t>
+  </si>
+  <si>
+    <t>a03a7c4</t>
+  </si>
+  <si>
+    <t>29cb315</t>
+  </si>
+  <si>
+    <t>ed63954</t>
+  </si>
+  <si>
+    <t>49d3346</t>
+  </si>
+  <si>
+    <t>4f4e5e5</t>
+  </si>
+  <si>
+    <t>b4c70a7</t>
+  </si>
+  <si>
+    <t>11eba3e</t>
+  </si>
+  <si>
+    <t>49c71cf</t>
+  </si>
+  <si>
+    <t>26faa6c</t>
+  </si>
+  <si>
+    <t>eecfdea</t>
+  </si>
+  <si>
+    <t>cd6ba17</t>
+  </si>
+  <si>
+    <t>2e660ce</t>
+  </si>
+  <si>
+    <t>76f0b77</t>
+  </si>
+  <si>
+    <t>252d119</t>
+  </si>
+  <si>
+    <t>a8b447b</t>
+  </si>
+  <si>
+    <t>26998c1</t>
+  </si>
+  <si>
+    <t>d285aad</t>
+  </si>
+  <si>
+    <t>aa9d44b</t>
+  </si>
+  <si>
+    <t>d748ba1</t>
+  </si>
+  <si>
+    <t>8254004</t>
+  </si>
+  <si>
+    <t>865beeb</t>
+  </si>
+  <si>
+    <t>f47495d</t>
+  </si>
+  <si>
+    <t>857f13c</t>
+  </si>
+  <si>
+    <t>english</t>
+  </si>
+  <si>
+    <t>japanese</t>
+  </si>
+  <si>
+    <t>BIRDS</t>
+  </si>
+  <si>
+    <t>CATS</t>
+  </si>
+  <si>
+    <t>DOGS</t>
+  </si>
+  <si>
+    <t>FISH</t>
+  </si>
+  <si>
+    <t>REPTILES</t>
+  </si>
+  <si>
+    <t>f1a7fca</t>
+  </si>
+  <si>
+    <t>403b0fb</t>
+  </si>
+  <si>
+    <t>c01d81b</t>
+  </si>
+  <si>
+    <t>cf3c4c6</t>
+  </si>
+  <si>
+    <t>c9fb7cf</t>
+  </si>
+  <si>
+    <t>d050262</t>
+  </si>
+  <si>
+    <t>7e8188d</t>
+  </si>
+  <si>
+    <t>daa7ab2</t>
+  </si>
+  <si>
+    <t>f646cda</t>
+  </si>
+  <si>
+    <t>1d87fe4</t>
+  </si>
+  <si>
+    <t>5eff8fa</t>
+  </si>
+  <si>
+    <t>6350c45</t>
+  </si>
+  <si>
+    <t>abc79df</t>
+  </si>
+  <si>
+    <t>038e5d7</t>
+  </si>
+  <si>
+    <t>0336baf</t>
+  </si>
+  <si>
+    <t>9b880e3</t>
+  </si>
+  <si>
+    <t>91301bb</t>
+  </si>
+  <si>
+    <t>cf3f433</t>
+  </si>
+  <si>
+    <t>741bd9e</t>
+  </si>
+  <si>
+    <t>de14995</t>
+  </si>
+  <si>
+    <t>c91e58d</t>
+  </si>
+  <si>
+    <t>dd70224</t>
+  </si>
+  <si>
+    <t>926e1d7</t>
+  </si>
+  <si>
+    <t>ba7494d</t>
+  </si>
+  <si>
+    <t>57619d7</t>
+  </si>
+  <si>
+    <t>ea467fc</t>
+  </si>
+  <si>
+    <t>99c30eb</t>
+  </si>
+  <si>
+    <t>7149706</t>
+  </si>
+  <si>
+    <t>c6c2675</t>
+  </si>
+  <si>
+    <t>e514a14</t>
+  </si>
+  <si>
+    <t>2d6fb02</t>
+  </si>
+  <si>
+    <t>c0383b4</t>
+  </si>
+  <si>
+    <t>7c4243a</t>
+  </si>
+  <si>
+    <t>e8bd25f</t>
+  </si>
+  <si>
+    <t>1fd5537</t>
+  </si>
+  <si>
+    <t>64e03bf</t>
+  </si>
+  <si>
+    <t>2fa8f9b</t>
+  </si>
+  <si>
+    <t>6d1e890</t>
+  </si>
+  <si>
+    <t>c6eeaf3</t>
+  </si>
+  <si>
+    <t>7528683</t>
+  </si>
+  <si>
+    <t>a23de8b</t>
+  </si>
+  <si>
+    <t>2bb354b</t>
+  </si>
+  <si>
+    <t>e664b98</t>
+  </si>
+  <si>
+    <t>14bc508</t>
+  </si>
+  <si>
+    <t>2244ad0</t>
+  </si>
+  <si>
+    <t>5ca2604</t>
+  </si>
+  <si>
+    <t>1bbf4aa</t>
+  </si>
+  <si>
+    <t>978a896</t>
+  </si>
+  <si>
+    <t>683fa8d</t>
+  </si>
+  <si>
+    <t>57257d2</t>
+  </si>
+  <si>
+    <t>adf954b</t>
+  </si>
+  <si>
+    <t>21cf39c</t>
+  </si>
+  <si>
+    <t>1df683c</t>
+  </si>
+  <si>
+    <t>a6af4d7</t>
+  </si>
+  <si>
+    <t>485b32c</t>
+  </si>
+  <si>
+    <t>f2652fd</t>
+  </si>
+  <si>
+    <t>1e64966</t>
+  </si>
+  <si>
+    <t>eef506c</t>
+  </si>
+  <si>
+    <t>fb3ab00</t>
+  </si>
+  <si>
+    <t>6cd724e</t>
+  </si>
+  <si>
+    <t>c80998c</t>
+  </si>
+  <si>
+    <t>04fd9f6</t>
+  </si>
+  <si>
+    <t>74d690f</t>
+  </si>
+  <si>
+    <t>21e6ee1</t>
+  </si>
+  <si>
+    <t>1917c99</t>
+  </si>
+  <si>
+    <t>780f71a</t>
+  </si>
+  <si>
+    <t>a8213b4</t>
+  </si>
+  <si>
+    <t>93fd0c0</t>
+  </si>
+  <si>
+    <t>88475c2</t>
+  </si>
+  <si>
+    <t>2db75bd</t>
+  </si>
+  <si>
+    <t>cd60b9a</t>
+  </si>
+  <si>
+    <t>2b70b57</t>
+  </si>
+  <si>
+    <t>849c121</t>
+  </si>
+  <si>
+    <t>2059e55</t>
+  </si>
+  <si>
+    <t>f321a34</t>
+  </si>
+  <si>
+    <t>59fdee9</t>
+  </si>
+  <si>
+    <t>d0b5b4c</t>
+  </si>
+  <si>
+    <t>4fb4e74</t>
+  </si>
+  <si>
+    <t>e8a4248</t>
+  </si>
+  <si>
+    <t>bbfa9ca</t>
+  </si>
+  <si>
+    <t>fa96098</t>
+  </si>
+  <si>
+    <t>3f34135</t>
+  </si>
+  <si>
+    <t>ff3ba44</t>
+  </si>
+  <si>
+    <t>682d895</t>
+  </si>
+  <si>
+    <t>8dd37fb</t>
+  </si>
+  <si>
+    <t>29e4f3f</t>
+  </si>
+  <si>
+    <t>c736286</t>
+  </si>
+  <si>
+    <t>a7da9a5</t>
+  </si>
+  <si>
+    <t>e5c7122</t>
+  </si>
+  <si>
+    <t>17499ad</t>
+  </si>
+  <si>
+    <t>8eb3be7</t>
+  </si>
+  <si>
+    <t>4b714b6</t>
+  </si>
+  <si>
+    <t>a3dd9c6</t>
+  </si>
+  <si>
+    <t>f215370</t>
+  </si>
+  <si>
+    <t>d2b73e0</t>
+  </si>
+  <si>
+    <t>07b5c6e</t>
+  </si>
+  <si>
+    <t>4baa922</t>
+  </si>
+  <si>
+    <t>8602565</t>
+  </si>
+  <si>
+    <t>2e8a273</t>
+  </si>
+  <si>
+    <t>2430695</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -1879,8 +2351,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="108" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="108.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1990,7 +2462,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -1998,11 +2470,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="17.28515625" style="3"/>
-    <col min="5" max="5" width="25.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="3"/>
-    <col min="7" max="7" width="27.42578125" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="17.28515625" style="3"/>
+    <col min="1" max="4" style="3" width="17.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="25.85546875" collapsed="true"/>
+    <col min="6" max="6" style="3" width="17.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="3" width="27.42578125" collapsed="true"/>
+    <col min="8" max="16384" style="3" width="17.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30.75" thickBot="1">
@@ -2044,8 +2516,8 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A2" s="4">
-        <v>1</v>
+      <c r="A2" s="4" t="s">
+        <v>572</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>14</v>
@@ -2080,10 +2552,16 @@
       <c r="L2" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M2" t="s">
+        <v>516</v>
+      </c>
+      <c r="N2" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="3" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A3" s="4">
-        <v>2</v>
+      <c r="A3" s="4" t="s">
+        <v>573</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>24</v>
@@ -2118,10 +2596,16 @@
       <c r="L3" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M3" t="s">
+        <v>515</v>
+      </c>
+      <c r="N3" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A4" s="7">
-        <v>3</v>
+      <c r="A4" s="7" t="s">
+        <v>574</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>33</v>
@@ -2156,10 +2640,16 @@
       <c r="L4" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M4" t="s">
+        <v>515</v>
+      </c>
+      <c r="N4" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A5" s="4">
-        <v>4</v>
+      <c r="A5" s="4" t="s">
+        <v>575</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>42</v>
@@ -2194,10 +2684,16 @@
       <c r="L5" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M5" t="s">
+        <v>515</v>
+      </c>
+      <c r="N5" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A6" s="4">
-        <v>5</v>
+      <c r="A6" s="4" t="s">
+        <v>576</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>51</v>
@@ -2232,10 +2728,16 @@
       <c r="L6" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M6" t="s">
+        <v>516</v>
+      </c>
+      <c r="N6" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A7" s="7">
-        <v>6</v>
+      <c r="A7" s="7" t="s">
+        <v>577</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>60</v>
@@ -2270,10 +2772,16 @@
       <c r="L7" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M7" t="s">
+        <v>515</v>
+      </c>
+      <c r="N7" t="s">
+        <v>519</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A8" s="4">
-        <v>7</v>
+      <c r="A8" s="4" t="s">
+        <v>578</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>69</v>
@@ -2308,10 +2816,16 @@
       <c r="L8" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N8" t="s">
+        <v>519</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A9" s="4">
-        <v>8</v>
+      <c r="A9" s="4" t="s">
+        <v>579</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>78</v>
@@ -2346,10 +2860,16 @@
       <c r="L9" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M9" t="s">
+        <v>515</v>
+      </c>
+      <c r="N9" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A10" s="7">
-        <v>9</v>
+      <c r="A10" s="7" t="s">
+        <v>580</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>87</v>
@@ -2384,10 +2904,16 @@
       <c r="L10" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M10" t="s">
+        <v>516</v>
+      </c>
+      <c r="N10" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A11" s="4">
-        <v>10</v>
+      <c r="A11" s="4" t="s">
+        <v>581</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>96</v>
@@ -2422,10 +2948,16 @@
       <c r="L11" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M11" t="s">
+        <v>516</v>
+      </c>
+      <c r="N11" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A12" s="4">
-        <v>11</v>
+      <c r="A12" s="4" t="s">
+        <v>582</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>105</v>
@@ -2460,10 +2992,16 @@
       <c r="L12" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M12" t="s">
+        <v>516</v>
+      </c>
+      <c r="N12" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A13" s="7">
-        <v>12</v>
+      <c r="A13" s="7" t="s">
+        <v>583</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>114</v>
@@ -2498,10 +3036,16 @@
       <c r="L13" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M13" t="s">
+        <v>515</v>
+      </c>
+      <c r="N13" t="s">
+        <v>519</v>
+      </c>
     </row>
     <row r="14" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A14" s="4">
-        <v>13</v>
+      <c r="A14" s="4" t="s">
+        <v>584</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>123</v>
@@ -2536,10 +3080,16 @@
       <c r="L14" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M14" t="s">
+        <v>515</v>
+      </c>
+      <c r="N14" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A15" s="4">
-        <v>14</v>
+      <c r="A15" s="4" t="s">
+        <v>585</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>131</v>
@@ -2574,10 +3124,16 @@
       <c r="L15" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M15" t="s">
+        <v>515</v>
+      </c>
+      <c r="N15" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="16" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A16" s="7">
-        <v>15</v>
+      <c r="A16" s="7" t="s">
+        <v>586</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>139</v>
@@ -2612,10 +3168,16 @@
       <c r="L16" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M16" t="s">
+        <v>515</v>
+      </c>
+      <c r="N16" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="17" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A17" s="4">
-        <v>16</v>
+      <c r="A17" s="4" t="s">
+        <v>587</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>148</v>
@@ -2650,10 +3212,16 @@
       <c r="L17" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M17" t="s">
+        <v>516</v>
+      </c>
+      <c r="N17" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="18" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A18" s="4">
-        <v>17</v>
+      <c r="A18" s="4" t="s">
+        <v>588</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>156</v>
@@ -2688,10 +3256,16 @@
       <c r="L18" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M18" t="s">
+        <v>515</v>
+      </c>
+      <c r="N18" t="s">
+        <v>519</v>
+      </c>
     </row>
     <row r="19" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A19" s="7">
-        <v>18</v>
+      <c r="A19" s="7" t="s">
+        <v>589</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>165</v>
@@ -2726,10 +3300,16 @@
       <c r="L19" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M19" t="s">
+        <v>515</v>
+      </c>
+      <c r="N19" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="20" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A20" s="4">
-        <v>19</v>
+      <c r="A20" s="4" t="s">
+        <v>590</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>173</v>
@@ -2764,10 +3344,16 @@
       <c r="L20" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M20" t="s">
+        <v>516</v>
+      </c>
+      <c r="N20" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="21" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A21" s="4">
-        <v>20</v>
+      <c r="A21" s="4" t="s">
+        <v>591</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>181</v>
@@ -2802,10 +3388,16 @@
       <c r="L21" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M21" t="s">
+        <v>515</v>
+      </c>
+      <c r="N21" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="22" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A22" s="7">
-        <v>21</v>
+      <c r="A22" s="7" t="s">
+        <v>592</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>190</v>
@@ -2840,10 +3432,16 @@
       <c r="L22" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M22" t="s">
+        <v>516</v>
+      </c>
+      <c r="N22" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="23" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A23" s="4">
-        <v>22</v>
+      <c r="A23" s="4" t="s">
+        <v>593</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>199</v>
@@ -2878,10 +3476,16 @@
       <c r="L23" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M23" t="s">
+        <v>515</v>
+      </c>
+      <c r="N23" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="24" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A24" s="4">
-        <v>23</v>
+      <c r="A24" s="4" t="s">
+        <v>594</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>207</v>
@@ -2916,10 +3520,16 @@
       <c r="L24" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M24" t="s">
+        <v>516</v>
+      </c>
+      <c r="N24" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="25" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A25" s="7">
-        <v>24</v>
+      <c r="A25" s="7" t="s">
+        <v>595</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>216</v>
@@ -2954,10 +3564,16 @@
       <c r="L25" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M25" t="s">
+        <v>516</v>
+      </c>
+      <c r="N25" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="26" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A26" s="4">
-        <v>25</v>
+      <c r="A26" s="4" t="s">
+        <v>596</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>225</v>
@@ -2992,10 +3608,16 @@
       <c r="L26" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M26" t="s">
+        <v>515</v>
+      </c>
+      <c r="N26" t="s">
+        <v>519</v>
+      </c>
     </row>
     <row r="27" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A27" s="4">
-        <v>26</v>
+      <c r="A27" s="4" t="s">
+        <v>597</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>234</v>
@@ -3030,10 +3652,16 @@
       <c r="L27" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M27" t="s">
+        <v>516</v>
+      </c>
+      <c r="N27" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="28" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A28" s="7">
-        <v>27</v>
+      <c r="A28" s="7" t="s">
+        <v>598</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>243</v>
@@ -3068,10 +3696,16 @@
       <c r="L28" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M28" t="s">
+        <v>515</v>
+      </c>
+      <c r="N28" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="29" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A29" s="4">
-        <v>28</v>
+      <c r="A29" s="4" t="s">
+        <v>599</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>251</v>
@@ -3106,10 +3740,16 @@
       <c r="L29" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M29" t="s">
+        <v>515</v>
+      </c>
+      <c r="N29" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="30" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A30" s="4">
-        <v>29</v>
+      <c r="A30" s="4" t="s">
+        <v>600</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>259</v>
@@ -3144,10 +3784,16 @@
       <c r="L30" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M30" t="s">
+        <v>515</v>
+      </c>
+      <c r="N30" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="31" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A31" s="7">
-        <v>30</v>
+      <c r="A31" s="7" t="s">
+        <v>601</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>268</v>
@@ -3182,10 +3828,16 @@
       <c r="L31" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M31" t="s">
+        <v>515</v>
+      </c>
+      <c r="N31" t="s">
+        <v>519</v>
+      </c>
     </row>
     <row r="32" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A32" s="4">
-        <v>31</v>
+      <c r="A32" s="4" t="s">
+        <v>602</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>276</v>
@@ -3220,10 +3872,16 @@
       <c r="L32" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M32" t="s">
+        <v>516</v>
+      </c>
+      <c r="N32" t="s">
+        <v>519</v>
+      </c>
     </row>
     <row r="33" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A33" s="4">
-        <v>32</v>
+      <c r="A33" s="4" t="s">
+        <v>603</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>284</v>
@@ -3258,10 +3916,16 @@
       <c r="L33" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M33" t="s">
+        <v>515</v>
+      </c>
+      <c r="N33" t="s">
+        <v>519</v>
+      </c>
     </row>
     <row r="34" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A34" s="7">
-        <v>33</v>
+      <c r="A34" s="7" t="s">
+        <v>604</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>292</v>
@@ -3296,10 +3960,16 @@
       <c r="L34" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M34" t="s">
+        <v>516</v>
+      </c>
+      <c r="N34" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="35" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A35" s="4">
-        <v>34</v>
+      <c r="A35" s="4" t="s">
+        <v>605</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>301</v>
@@ -3334,10 +4004,16 @@
       <c r="L35" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M35" t="s">
+        <v>515</v>
+      </c>
+      <c r="N35" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="36" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A36" s="4">
-        <v>35</v>
+      <c r="A36" s="4" t="s">
+        <v>606</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>310</v>
@@ -3372,10 +4048,16 @@
       <c r="L36" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M36" t="s">
+        <v>515</v>
+      </c>
+      <c r="N36" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="37" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A37" s="7">
-        <v>36</v>
+      <c r="A37" s="7" t="s">
+        <v>607</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>319</v>
@@ -3410,10 +4092,16 @@
       <c r="L37" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M37" t="s">
+        <v>515</v>
+      </c>
+      <c r="N37" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="38" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A38" s="4">
-        <v>37</v>
+      <c r="A38" s="4" t="s">
+        <v>608</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>327</v>
@@ -3448,10 +4136,16 @@
       <c r="L38" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M38" t="s">
+        <v>516</v>
+      </c>
+      <c r="N38" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="39" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A39" s="4">
-        <v>38</v>
+      <c r="A39" s="4" t="s">
+        <v>609</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>336</v>
@@ -3486,10 +4180,16 @@
       <c r="L39" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M39" t="s">
+        <v>515</v>
+      </c>
+      <c r="N39" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="40" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A40" s="7">
-        <v>39</v>
+      <c r="A40" s="7" t="s">
+        <v>610</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>344</v>
@@ -3524,10 +4224,16 @@
       <c r="L40" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M40" t="s">
+        <v>516</v>
+      </c>
+      <c r="N40" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="41" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A41" s="4">
-        <v>40</v>
+      <c r="A41" s="4" t="s">
+        <v>611</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>352</v>
@@ -3562,10 +4268,16 @@
       <c r="L41" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M41" t="s">
+        <v>516</v>
+      </c>
+      <c r="N41" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="42" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A42" s="4">
-        <v>41</v>
+      <c r="A42" s="4" t="s">
+        <v>612</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>360</v>
@@ -3600,10 +4312,16 @@
       <c r="L42" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M42" t="s">
+        <v>516</v>
+      </c>
+      <c r="N42" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="43" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A43" s="7">
-        <v>42</v>
+      <c r="A43" s="7" t="s">
+        <v>613</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>368</v>
@@ -3638,10 +4356,16 @@
       <c r="L43" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M43" t="s">
+        <v>515</v>
+      </c>
+      <c r="N43" t="s">
+        <v>519</v>
+      </c>
     </row>
     <row r="44" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A44" s="4">
-        <v>43</v>
+      <c r="A44" s="4" t="s">
+        <v>614</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>377</v>
@@ -3676,10 +4400,16 @@
       <c r="L44" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M44" t="s">
+        <v>516</v>
+      </c>
+      <c r="N44" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="45" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A45" s="4">
-        <v>44</v>
+      <c r="A45" s="4" t="s">
+        <v>615</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>386</v>
@@ -3714,10 +4444,16 @@
       <c r="L45" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M45" t="s">
+        <v>515</v>
+      </c>
+      <c r="N45" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="46" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A46" s="7">
-        <v>45</v>
+      <c r="A46" s="7" t="s">
+        <v>616</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>394</v>
@@ -3752,10 +4488,16 @@
       <c r="L46" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M46" t="s">
+        <v>516</v>
+      </c>
+      <c r="N46" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="47" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A47" s="4">
-        <v>46</v>
+      <c r="A47" s="4" t="s">
+        <v>617</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>402</v>
@@ -3790,10 +4532,16 @@
       <c r="L47" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M47" t="s">
+        <v>516</v>
+      </c>
+      <c r="N47" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="48" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A48" s="4">
-        <v>47</v>
+      <c r="A48" s="4" t="s">
+        <v>618</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>410</v>
@@ -3828,10 +4576,16 @@
       <c r="L48" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M48" t="s">
+        <v>516</v>
+      </c>
+      <c r="N48" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="49" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A49" s="7">
-        <v>48</v>
+      <c r="A49" s="7" t="s">
+        <v>619</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>418</v>
@@ -3866,10 +4620,16 @@
       <c r="L49" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M49" t="s">
+        <v>515</v>
+      </c>
+      <c r="N49" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="50" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A50" s="4">
-        <v>49</v>
+      <c r="A50" s="4" t="s">
+        <v>620</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>427</v>
@@ -3904,10 +4664,16 @@
       <c r="L50" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M50" t="s">
+        <v>515</v>
+      </c>
+      <c r="N50" t="s">
+        <v>519</v>
+      </c>
     </row>
     <row r="51" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A51" s="4">
-        <v>50</v>
+      <c r="A51" s="4" t="s">
+        <v>621</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>436</v>
@@ -3941,6 +4707,12 @@
       </c>
       <c r="L51" s="5" t="s">
         <v>23</v>
+      </c>
+      <c r="M51" t="s">
+        <v>515</v>
+      </c>
+      <c r="N51" t="s">
+        <v>520</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test runs and data
</commit_message>
<xml_diff>
--- a/FirstProject/data/pet-store-data.xlsx
+++ b/FirstProject/data/pet-store-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="772">
   <si>
     <t>ITEM_ID</t>
   </si>
@@ -1881,6 +1881,456 @@
   </si>
   <si>
     <t>2430695</t>
+  </si>
+  <si>
+    <t>1a3479f</t>
+  </si>
+  <si>
+    <t>8df5c1d</t>
+  </si>
+  <si>
+    <t>c8c2310</t>
+  </si>
+  <si>
+    <t>760a09f</t>
+  </si>
+  <si>
+    <t>c0cb3d3</t>
+  </si>
+  <si>
+    <t>ec0b8db</t>
+  </si>
+  <si>
+    <t>6474db6</t>
+  </si>
+  <si>
+    <t>e4d4d9a</t>
+  </si>
+  <si>
+    <t>1d51d6c</t>
+  </si>
+  <si>
+    <t>825a4a0</t>
+  </si>
+  <si>
+    <t>59da995</t>
+  </si>
+  <si>
+    <t>aac1c98</t>
+  </si>
+  <si>
+    <t>7437457</t>
+  </si>
+  <si>
+    <t>cd487d3</t>
+  </si>
+  <si>
+    <t>4bfbd77</t>
+  </si>
+  <si>
+    <t>e9986c7</t>
+  </si>
+  <si>
+    <t>df9a455</t>
+  </si>
+  <si>
+    <t>ca834d7</t>
+  </si>
+  <si>
+    <t>e91fb21</t>
+  </si>
+  <si>
+    <t>4438459</t>
+  </si>
+  <si>
+    <t>2bfc95b</t>
+  </si>
+  <si>
+    <t>47c490e</t>
+  </si>
+  <si>
+    <t>45819cd</t>
+  </si>
+  <si>
+    <t>a81e2a2</t>
+  </si>
+  <si>
+    <t>31adb66</t>
+  </si>
+  <si>
+    <t>41bfc6e</t>
+  </si>
+  <si>
+    <t>c04f36a</t>
+  </si>
+  <si>
+    <t>b9c0f5f</t>
+  </si>
+  <si>
+    <t>54c8a95</t>
+  </si>
+  <si>
+    <t>818a02b</t>
+  </si>
+  <si>
+    <t>6a7b961</t>
+  </si>
+  <si>
+    <t>d68a0e6</t>
+  </si>
+  <si>
+    <t>086e8f2</t>
+  </si>
+  <si>
+    <t>abcd8c2</t>
+  </si>
+  <si>
+    <t>18b58e0</t>
+  </si>
+  <si>
+    <t>51cc075</t>
+  </si>
+  <si>
+    <t>6be9fdd</t>
+  </si>
+  <si>
+    <t>5dfcf18</t>
+  </si>
+  <si>
+    <t>7d6b04e</t>
+  </si>
+  <si>
+    <t>1b69994</t>
+  </si>
+  <si>
+    <t>d91ca55</t>
+  </si>
+  <si>
+    <t>48c2ef5</t>
+  </si>
+  <si>
+    <t>23cf30e</t>
+  </si>
+  <si>
+    <t>1871bf8</t>
+  </si>
+  <si>
+    <t>2960769</t>
+  </si>
+  <si>
+    <t>f4c5291</t>
+  </si>
+  <si>
+    <t>580f0e7</t>
+  </si>
+  <si>
+    <t>1389f2c</t>
+  </si>
+  <si>
+    <t>db4fffe</t>
+  </si>
+  <si>
+    <t>ea4491d</t>
+  </si>
+  <si>
+    <t>4cb925e</t>
+  </si>
+  <si>
+    <t>de09935</t>
+  </si>
+  <si>
+    <t>8304bdb</t>
+  </si>
+  <si>
+    <t>fe8b61e</t>
+  </si>
+  <si>
+    <t>7d5153e</t>
+  </si>
+  <si>
+    <t>c85a245</t>
+  </si>
+  <si>
+    <t>fc5530f</t>
+  </si>
+  <si>
+    <t>653bba1</t>
+  </si>
+  <si>
+    <t>71233b1</t>
+  </si>
+  <si>
+    <t>54898b6</t>
+  </si>
+  <si>
+    <t>38edc1d</t>
+  </si>
+  <si>
+    <t>889ef47</t>
+  </si>
+  <si>
+    <t>94c7319</t>
+  </si>
+  <si>
+    <t>44763ff</t>
+  </si>
+  <si>
+    <t>8ecc2bc</t>
+  </si>
+  <si>
+    <t>e10a707</t>
+  </si>
+  <si>
+    <t>6b42a83</t>
+  </si>
+  <si>
+    <t>0dc8875</t>
+  </si>
+  <si>
+    <t>4e5598e</t>
+  </si>
+  <si>
+    <t>c580068</t>
+  </si>
+  <si>
+    <t>2d55972</t>
+  </si>
+  <si>
+    <t>2042f89</t>
+  </si>
+  <si>
+    <t>f4ab561</t>
+  </si>
+  <si>
+    <t>e7f0f9d</t>
+  </si>
+  <si>
+    <t>7d63bb2</t>
+  </si>
+  <si>
+    <t>89684db</t>
+  </si>
+  <si>
+    <t>8e3d16c</t>
+  </si>
+  <si>
+    <t>051a848</t>
+  </si>
+  <si>
+    <t>346f147</t>
+  </si>
+  <si>
+    <t>521f236</t>
+  </si>
+  <si>
+    <t>2cf77ff</t>
+  </si>
+  <si>
+    <t>00b3600</t>
+  </si>
+  <si>
+    <t>685a197</t>
+  </si>
+  <si>
+    <t>4828b11</t>
+  </si>
+  <si>
+    <t>715e640</t>
+  </si>
+  <si>
+    <t>98a1e71</t>
+  </si>
+  <si>
+    <t>ee71c2c</t>
+  </si>
+  <si>
+    <t>5170087</t>
+  </si>
+  <si>
+    <t>e397531</t>
+  </si>
+  <si>
+    <t>bfb7a72</t>
+  </si>
+  <si>
+    <t>2b02c10</t>
+  </si>
+  <si>
+    <t>3e65888</t>
+  </si>
+  <si>
+    <t>3712ef3</t>
+  </si>
+  <si>
+    <t>0c263b9</t>
+  </si>
+  <si>
+    <t>4fa2fd8</t>
+  </si>
+  <si>
+    <t>170d8ad</t>
+  </si>
+  <si>
+    <t>4394c5a</t>
+  </si>
+  <si>
+    <t>1f6a2d8</t>
+  </si>
+  <si>
+    <t>7d7a8b7</t>
+  </si>
+  <si>
+    <t>ed1f60b</t>
+  </si>
+  <si>
+    <t>c36c75c</t>
+  </si>
+  <si>
+    <t>092adc4</t>
+  </si>
+  <si>
+    <t>210be5a</t>
+  </si>
+  <si>
+    <t>1e90dc1</t>
+  </si>
+  <si>
+    <t>b71efee</t>
+  </si>
+  <si>
+    <t>2109cf6</t>
+  </si>
+  <si>
+    <t>8ffc71d</t>
+  </si>
+  <si>
+    <t>1aa5347</t>
+  </si>
+  <si>
+    <t>e794a78</t>
+  </si>
+  <si>
+    <t>4d49497</t>
+  </si>
+  <si>
+    <t>d9cf7b8</t>
+  </si>
+  <si>
+    <t>0da479a</t>
+  </si>
+  <si>
+    <t>1563471</t>
+  </si>
+  <si>
+    <t>cea858b</t>
+  </si>
+  <si>
+    <t>2ebb06c</t>
+  </si>
+  <si>
+    <t>53316bd</t>
+  </si>
+  <si>
+    <t>e190b2e</t>
+  </si>
+  <si>
+    <t>1449692</t>
+  </si>
+  <si>
+    <t>2b2f079</t>
+  </si>
+  <si>
+    <t>b6ca709</t>
+  </si>
+  <si>
+    <t>d28a183</t>
+  </si>
+  <si>
+    <t>bbde1e0</t>
+  </si>
+  <si>
+    <t>ff6247c</t>
+  </si>
+  <si>
+    <t>3f9ea5e</t>
+  </si>
+  <si>
+    <t>ef6dac0</t>
+  </si>
+  <si>
+    <t>e5d3fce</t>
+  </si>
+  <si>
+    <t>a046401</t>
+  </si>
+  <si>
+    <t>eb0c5b1</t>
+  </si>
+  <si>
+    <t>66e82a2</t>
+  </si>
+  <si>
+    <t>c86a4e2</t>
+  </si>
+  <si>
+    <t>abd949b</t>
+  </si>
+  <si>
+    <t>f7f0091</t>
+  </si>
+  <si>
+    <t>c4fc0c8</t>
+  </si>
+  <si>
+    <t>78e02fc</t>
+  </si>
+  <si>
+    <t>1d3dd2f</t>
+  </si>
+  <si>
+    <t>dce69c2</t>
+  </si>
+  <si>
+    <t>6cb08c9</t>
+  </si>
+  <si>
+    <t>1e4d2c6</t>
+  </si>
+  <si>
+    <t>9385d98</t>
+  </si>
+  <si>
+    <t>5082b96</t>
+  </si>
+  <si>
+    <t>7585309</t>
+  </si>
+  <si>
+    <t>5437757</t>
+  </si>
+  <si>
+    <t>7722a75</t>
+  </si>
+  <si>
+    <t>0cf1d93</t>
+  </si>
+  <si>
+    <t>a0bbc2c</t>
+  </si>
+  <si>
+    <t>f1f15dd</t>
+  </si>
+  <si>
+    <t>d5dce40</t>
+  </si>
+  <si>
+    <t>b5601e4</t>
+  </si>
+  <si>
+    <t>a123e52</t>
+  </si>
+  <si>
+    <t>a49811b</t>
   </si>
 </sst>
 </file>
@@ -2517,7 +2967,7 @@
     </row>
     <row r="2" spans="1:12" ht="44.25" thickBot="1">
       <c r="A2" s="4" t="s">
-        <v>572</v>
+        <v>722</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>14</v>
@@ -2556,12 +3006,12 @@
         <v>516</v>
       </c>
       <c r="N2" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="44.25" thickBot="1">
       <c r="A3" s="4" t="s">
-        <v>573</v>
+        <v>723</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>24</v>
@@ -2597,7 +3047,7 @@
         <v>23</v>
       </c>
       <c r="M3" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="N3" t="s">
         <v>518</v>
@@ -2605,7 +3055,7 @@
     </row>
     <row r="4" spans="1:12" ht="58.5" thickBot="1">
       <c r="A4" s="7" t="s">
-        <v>574</v>
+        <v>724</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>33</v>
@@ -2641,15 +3091,15 @@
         <v>23</v>
       </c>
       <c r="M4" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="N4" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="58.5" thickBot="1">
       <c r="A5" s="4" t="s">
-        <v>575</v>
+        <v>725</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>42</v>
@@ -2685,15 +3135,15 @@
         <v>23</v>
       </c>
       <c r="M5" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="N5" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="44.25" thickBot="1">
       <c r="A6" s="4" t="s">
-        <v>576</v>
+        <v>726</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>51</v>
@@ -2732,12 +3182,12 @@
         <v>516</v>
       </c>
       <c r="N6" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="44.25" thickBot="1">
       <c r="A7" s="7" t="s">
-        <v>577</v>
+        <v>727</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>60</v>
@@ -2776,12 +3226,12 @@
         <v>515</v>
       </c>
       <c r="N7" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="44.25" thickBot="1">
       <c r="A8" s="4" t="s">
-        <v>578</v>
+        <v>728</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>69</v>
@@ -2820,12 +3270,12 @@
         <v>515</v>
       </c>
       <c r="N8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="44.25" thickBot="1">
       <c r="A9" s="4" t="s">
-        <v>579</v>
+        <v>729</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>78</v>
@@ -2864,12 +3314,12 @@
         <v>515</v>
       </c>
       <c r="N9" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="58.5" thickBot="1">
       <c r="A10" s="7" t="s">
-        <v>580</v>
+        <v>730</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>87</v>
@@ -2908,12 +3358,12 @@
         <v>516</v>
       </c>
       <c r="N10" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="58.5" thickBot="1">
       <c r="A11" s="4" t="s">
-        <v>581</v>
+        <v>731</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>96</v>
@@ -2952,12 +3402,12 @@
         <v>516</v>
       </c>
       <c r="N11" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="58.5" thickBot="1">
       <c r="A12" s="4" t="s">
-        <v>582</v>
+        <v>732</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>105</v>
@@ -2996,12 +3446,12 @@
         <v>516</v>
       </c>
       <c r="N12" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="44.25" thickBot="1">
       <c r="A13" s="7" t="s">
-        <v>583</v>
+        <v>733</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>114</v>
@@ -3045,7 +3495,7 @@
     </row>
     <row r="14" spans="1:12" ht="44.25" thickBot="1">
       <c r="A14" s="4" t="s">
-        <v>584</v>
+        <v>734</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>123</v>
@@ -3081,15 +3531,15 @@
         <v>23</v>
       </c>
       <c r="M14" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="N14" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="44.25" thickBot="1">
       <c r="A15" s="4" t="s">
-        <v>585</v>
+        <v>735</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>131</v>
@@ -3128,12 +3578,12 @@
         <v>515</v>
       </c>
       <c r="N15" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="44.25" thickBot="1">
       <c r="A16" s="7" t="s">
-        <v>586</v>
+        <v>736</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>139</v>
@@ -3172,12 +3622,12 @@
         <v>515</v>
       </c>
       <c r="N16" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="44.25" thickBot="1">
       <c r="A17" s="4" t="s">
-        <v>587</v>
+        <v>737</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>148</v>
@@ -3216,12 +3666,12 @@
         <v>516</v>
       </c>
       <c r="N17" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="44.25" thickBot="1">
       <c r="A18" s="4" t="s">
-        <v>588</v>
+        <v>738</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>156</v>
@@ -3260,12 +3710,12 @@
         <v>515</v>
       </c>
       <c r="N18" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="44.25" thickBot="1">
       <c r="A19" s="7" t="s">
-        <v>589</v>
+        <v>739</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>165</v>
@@ -3301,7 +3751,7 @@
         <v>23</v>
       </c>
       <c r="M19" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="N19" t="s">
         <v>521</v>
@@ -3309,7 +3759,7 @@
     </row>
     <row r="20" spans="1:12" ht="44.25" thickBot="1">
       <c r="A20" s="4" t="s">
-        <v>590</v>
+        <v>740</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>173</v>
@@ -3348,12 +3798,12 @@
         <v>516</v>
       </c>
       <c r="N20" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="44.25" thickBot="1">
       <c r="A21" s="4" t="s">
-        <v>591</v>
+        <v>741</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>181</v>
@@ -3392,12 +3842,12 @@
         <v>515</v>
       </c>
       <c r="N21" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="44.25" thickBot="1">
       <c r="A22" s="7" t="s">
-        <v>592</v>
+        <v>742</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>190</v>
@@ -3436,12 +3886,12 @@
         <v>516</v>
       </c>
       <c r="N22" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="58.5" thickBot="1">
       <c r="A23" s="4" t="s">
-        <v>593</v>
+        <v>743</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>199</v>
@@ -3477,15 +3927,15 @@
         <v>23</v>
       </c>
       <c r="M23" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="N23" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="44.25" thickBot="1">
       <c r="A24" s="4" t="s">
-        <v>594</v>
+        <v>744</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>207</v>
@@ -3521,15 +3971,15 @@
         <v>23</v>
       </c>
       <c r="M24" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="N24" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="58.5" thickBot="1">
       <c r="A25" s="7" t="s">
-        <v>595</v>
+        <v>745</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>216</v>
@@ -3568,12 +4018,12 @@
         <v>516</v>
       </c>
       <c r="N25" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="58.5" thickBot="1">
       <c r="A26" s="4" t="s">
-        <v>596</v>
+        <v>746</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>225</v>
@@ -3612,12 +4062,12 @@
         <v>515</v>
       </c>
       <c r="N26" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="58.5" thickBot="1">
       <c r="A27" s="4" t="s">
-        <v>597</v>
+        <v>747</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>234</v>
@@ -3653,15 +4103,15 @@
         <v>23</v>
       </c>
       <c r="M27" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="N27" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="44.25" thickBot="1">
       <c r="A28" s="7" t="s">
-        <v>598</v>
+        <v>748</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>243</v>
@@ -3697,15 +4147,15 @@
         <v>23</v>
       </c>
       <c r="M28" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="N28" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="58.5" thickBot="1">
       <c r="A29" s="4" t="s">
-        <v>599</v>
+        <v>749</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>251</v>
@@ -3741,7 +4191,7 @@
         <v>23</v>
       </c>
       <c r="M29" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="N29" t="s">
         <v>520</v>
@@ -3749,7 +4199,7 @@
     </row>
     <row r="30" spans="1:12" ht="44.25" thickBot="1">
       <c r="A30" s="4" t="s">
-        <v>600</v>
+        <v>750</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>259</v>
@@ -3788,12 +4238,12 @@
         <v>515</v>
       </c>
       <c r="N30" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="58.5" thickBot="1">
       <c r="A31" s="7" t="s">
-        <v>601</v>
+        <v>751</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>268</v>
@@ -3829,15 +4279,15 @@
         <v>23</v>
       </c>
       <c r="M31" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="N31" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="44.25" thickBot="1">
       <c r="A32" s="4" t="s">
-        <v>602</v>
+        <v>752</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>276</v>
@@ -3873,7 +4323,7 @@
         <v>23</v>
       </c>
       <c r="M32" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="N32" t="s">
         <v>519</v>
@@ -3881,7 +4331,7 @@
     </row>
     <row r="33" spans="1:12" ht="58.5" thickBot="1">
       <c r="A33" s="4" t="s">
-        <v>603</v>
+        <v>753</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>284</v>
@@ -3917,15 +4367,15 @@
         <v>23</v>
       </c>
       <c r="M33" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="N33" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="44.25" thickBot="1">
       <c r="A34" s="7" t="s">
-        <v>604</v>
+        <v>754</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>292</v>
@@ -3969,7 +4419,7 @@
     </row>
     <row r="35" spans="1:12" ht="58.5" thickBot="1">
       <c r="A35" s="4" t="s">
-        <v>605</v>
+        <v>755</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>301</v>
@@ -4005,7 +4455,7 @@
         <v>23</v>
       </c>
       <c r="M35" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="N35" t="s">
         <v>517</v>
@@ -4013,7 +4463,7 @@
     </row>
     <row r="36" spans="1:12" ht="58.5" thickBot="1">
       <c r="A36" s="4" t="s">
-        <v>606</v>
+        <v>756</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>310</v>
@@ -4049,15 +4499,15 @@
         <v>23</v>
       </c>
       <c r="M36" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="N36" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="44.25" thickBot="1">
       <c r="A37" s="7" t="s">
-        <v>607</v>
+        <v>757</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>319</v>
@@ -4096,12 +4546,12 @@
         <v>515</v>
       </c>
       <c r="N37" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="44.25" thickBot="1">
       <c r="A38" s="4" t="s">
-        <v>608</v>
+        <v>758</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>327</v>
@@ -4137,15 +4587,15 @@
         <v>23</v>
       </c>
       <c r="M38" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="N38" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="58.5" thickBot="1">
       <c r="A39" s="4" t="s">
-        <v>609</v>
+        <v>759</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>336</v>
@@ -4181,15 +4631,15 @@
         <v>23</v>
       </c>
       <c r="M39" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="N39" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="44.25" thickBot="1">
       <c r="A40" s="7" t="s">
-        <v>610</v>
+        <v>760</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>344</v>
@@ -4225,15 +4675,15 @@
         <v>23</v>
       </c>
       <c r="M40" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="N40" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="44.25" thickBot="1">
       <c r="A41" s="4" t="s">
-        <v>611</v>
+        <v>761</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>352</v>
@@ -4269,15 +4719,15 @@
         <v>23</v>
       </c>
       <c r="M41" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="N41" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="58.5" thickBot="1">
       <c r="A42" s="4" t="s">
-        <v>612</v>
+        <v>762</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>360</v>
@@ -4313,15 +4763,15 @@
         <v>23</v>
       </c>
       <c r="M42" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="N42" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="44.25" thickBot="1">
       <c r="A43" s="7" t="s">
-        <v>613</v>
+        <v>763</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>368</v>
@@ -4357,7 +4807,7 @@
         <v>23</v>
       </c>
       <c r="M43" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="N43" t="s">
         <v>519</v>
@@ -4365,7 +4815,7 @@
     </row>
     <row r="44" spans="1:12" ht="58.5" thickBot="1">
       <c r="A44" s="4" t="s">
-        <v>614</v>
+        <v>764</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>377</v>
@@ -4401,15 +4851,15 @@
         <v>23</v>
       </c>
       <c r="M44" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="N44" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="58.5" thickBot="1">
       <c r="A45" s="4" t="s">
-        <v>615</v>
+        <v>765</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>386</v>
@@ -4448,12 +4898,12 @@
         <v>515</v>
       </c>
       <c r="N45" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="44.25" thickBot="1">
       <c r="A46" s="7" t="s">
-        <v>616</v>
+        <v>766</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>394</v>
@@ -4489,15 +4939,15 @@
         <v>23</v>
       </c>
       <c r="M46" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="N46" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="58.5" thickBot="1">
       <c r="A47" s="4" t="s">
-        <v>617</v>
+        <v>767</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>402</v>
@@ -4536,12 +4986,12 @@
         <v>516</v>
       </c>
       <c r="N47" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="44.25" thickBot="1">
       <c r="A48" s="4" t="s">
-        <v>618</v>
+        <v>768</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>410</v>
@@ -4577,15 +5027,15 @@
         <v>23</v>
       </c>
       <c r="M48" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="N48" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="44.25" thickBot="1">
       <c r="A49" s="7" t="s">
-        <v>619</v>
+        <v>769</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>418</v>
@@ -4629,7 +5079,7 @@
     </row>
     <row r="50" spans="1:12" ht="44.25" thickBot="1">
       <c r="A50" s="4" t="s">
-        <v>620</v>
+        <v>770</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>427</v>
@@ -4668,12 +5118,12 @@
         <v>515</v>
       </c>
       <c r="N50" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="44.25" thickBot="1">
       <c r="A51" s="4" t="s">
-        <v>621</v>
+        <v>771</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>436</v>
@@ -4709,10 +5159,10 @@
         <v>23</v>
       </c>
       <c r="M51" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="N51" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
   </sheetData>

</xml_diff>